<commit_message>
add planning info and incorperate edits
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B04D2A-7CF2-4171-A784-A40BF06B1572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA20117-3166-4F15-8BFD-B535FBDFD35A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -645,6 +645,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="12" max="12" width="28.875" customWidth="1"/>
     <col min="13" max="13" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
version 1.1, fix error in priorities comment, change app titles, clarify survey extent as upstream only  in summary table
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC5D6D8-4360-475E-83A0-430AAE87F27A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C96496-01EC-450D-AC16-2C40979ABBE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -242,9 +242,6 @@
     <t>Good flows, pools to 0.6m deep and pockets of gravel suitable for spawning. Infrequent large woody debris jams to 0.5m high.  Sites electrofished upstream and downstream with one bull trout captured downstream within 315m site.</t>
   </si>
   <si>
-    <t>Deep pools, large woody debris and boulders present.  Habitat quality decreases with distance upstream.  Upstream tributary too steep at 250m upstream.  Channel is Grave Creek mainstem that has redirected from historic channel. Culvert is 170m usptream of 62425.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Good flows, pools to 0.6m deep and pockets of gravel suitable for salmonid spawning throughout.  Infrequent large woody debris jams to 0.5m high.  Electrofishing indicated generally higher densities of fry, parr and juvenile westslope cutthrout trout downstream when compared to upstream. </t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>WCT</t>
   </si>
   <si>
-    <t>Undercut banks, small woody debris, large woody debris, boulders, deep pools, and overhanging vegetation present.  Abundant gravels present. Habitat  increasingly complex upstream. Watershed is a habitat protection area with motor vehicle restrictions. Elk Valley Park recreation site is located downstream of the crossing.</t>
-  </si>
-  <si>
     <t>A 4.4m high chute was located 200m downstream of crossing (UTM: 11U 668858 5481210) and is considered a permanent impassable barrier to upstream migration.</t>
   </si>
   <si>
@@ -275,10 +269,16 @@
     <t>Abundant gravels suitable for resident and fluvial westslope cutthrout trout spawning.  Frequent pools to 40cm deep associated with woody debris.  Within old growth cedar forest and not mapped in the freshwater atlas stream layer.  Flows potentially diverted  as part of a micro-hydro facilty for Island Lake Lodge.</t>
   </si>
   <si>
-    <t xml:space="preserve">Boulders, small woody debris, large woody debris, undercut banks, overhanging vegetation and gravels suitable for spawning.  Electrofished upstream and downstream of the crossing with westslope cutthrout trout fry, juvenile and adult fish observed downstream only.  Densities of parr lower in the steeper habitat located upstream. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Undercut banks throughout with small woody debris, large woody debris, deep pools, and overhanging vegetation also present.  Abundant gravels suitable for resident westslope cutthrout trout spawning. Fry observed upstream and downstream. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boulders, small woody debris, large woody debris, undercut banks, overhanging vegetation and gravels suitable for spawning.  Electrofished upstream and downstream of the crossing with westslope cutthrout trout fry, juvenile and adult fish captured downstream and only parr captured upstream.  Density of parr (fish/area) lower in the steeper habitat located upstream. </t>
+  </si>
+  <si>
+    <t>Deep pools, large woody debris and boulders present.  Habitat quality decreases with distance upstream.  Upstream tributary too steep at 250m upstream.  Channel is Grave Creek mainstem that has redirected from historic channel. Located 170m usptream of 62425.</t>
+  </si>
+  <si>
+    <t>Undercut banks, small woody debris, large woody debris, boulders, deep pools, and overhanging vegetation present.  Abundant gravels present. Habitat  increasingly complex upstream. Watershed is a habitat protection area with motor vehicle restrictions. Elk Valley Park recreation site is located downstream of the crossing. Water too cold to sample. Recommend fish sampling upstream and down.</t>
   </si>
 </sst>
 </file>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -878,7 +878,7 @@
         <v>2300</v>
       </c>
       <c r="M9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -901,13 +901,13 @@
         <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="L10">
         <v>1800</v>
       </c>
       <c r="M10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -936,7 +936,7 @@
         <v>170</v>
       </c>
       <c r="M11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>44</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L13">
         <v>350</v>
@@ -1025,7 +1025,7 @@
         <v>44</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L15">
         <v>1800</v>
@@ -1077,7 +1077,7 @@
         <v>29</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L17">
         <v>4500</v>
@@ -1126,13 +1126,13 @@
         <v>44</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L19">
         <v>540</v>
       </c>
       <c r="M19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N19" t="s">
         <v>9</v>
@@ -1178,13 +1178,13 @@
         <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L21">
         <v>7200</v>
       </c>
       <c r="M21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1241,13 +1241,13 @@
         <v>29</v>
       </c>
       <c r="J24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L24">
         <v>515</v>
       </c>
       <c r="M24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1287,13 +1287,13 @@
         <v>29</v>
       </c>
       <c r="J26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L26">
         <v>2700</v>
       </c>
       <c r="M26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
         <v>29</v>
       </c>
       <c r="J28" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="L28">
         <v>11600</v>
@@ -1376,7 +1376,7 @@
         <v>62</v>
       </c>
       <c r="J30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L30">
         <v>0</v>

</xml_diff>